<commit_message>
Fix: change Slovenian code from si to sl [IDEC-302]
</commit_message>
<xml_diff>
--- a/i18n/excel_from_translation/adas.dss.xlsx
+++ b/i18n/excel_from_translation/adas.dss.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26014"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rskgroup.sharepoint.com/sites/IPMDecisions274/Shared Documents/WP2/Translation files/Release-2022-12/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1063" documentId="11_E2FBB6334E2F4B8581BA093A4E4ED1A8A548824E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7AC1AE77-F7C2-403D-A4A2-C365049C3309}"/>
+  <xr:revisionPtr revIDLastSave="1071" documentId="11_E2FBB6334E2F4B8581BA093A4E4ED1A8A548824E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2682E67D-810A-4963-904F-F82109BE3520}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" firstSheet="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -168,7 +168,7 @@
     <t>nl</t>
   </si>
   <si>
-    <t>si</t>
+    <t>sl</t>
   </si>
   <si>
     <t>adas.dss.0_0_4.name</t>
@@ -7913,7 +7913,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
@@ -7977,8 +7977,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P40"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="15"/>
@@ -9228,7 +9228,7 @@
   <dimension ref="A1:P58"/>
   <sheetViews>
     <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
@@ -10213,8 +10213,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:P35"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
@@ -11549,8 +11549,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:P27"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
@@ -12389,8 +12389,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:P26"/>
   <sheetViews>
-    <sheetView topLeftCell="C7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
@@ -13195,8 +13195,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:P35"/>
   <sheetViews>
-    <sheetView topLeftCell="D8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
@@ -14362,8 +14362,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:P30"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
@@ -15264,6 +15264,28 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="49b2234f-12e0-4bdf-b627-3d078507bec9" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="f0f33890-2782-435d-9951-89eaf76ec08c">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CE6F8D6BD046F944849C04732F5FA09C" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="985394bff33c465c59c1b6ffc7f2b18c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="f0f33890-2782-435d-9951-89eaf76ec08c" xmlns:ns3="49b2234f-12e0-4bdf-b627-3d078507bec9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e6e7ee76b1c64bbcff38e34ea77f7800" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -15523,30 +15545,8 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="49b2234f-12e0-4bdf-b627-3d078507bec9" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="f0f33890-2782-435d-9951-89eaf76ec08c">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C777E8D5-A886-4028-BCA2-CDB3C6FF63CD}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5ACB3F0D-A741-4B65-9224-F227206A784E}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -15554,5 +15554,5 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5ACB3F0D-A741-4B65-9224-F227206A784E}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C777E8D5-A886-4028-BCA2-CDB3C6FF63CD}"/>
 </file>
</xml_diff>